<commit_message>
WIPStock--change In View MaterialConversion--insert,update delete function Jobworkopening--add validation for dublicate partcode
</commit_message>
<xml_diff>
--- a/eTactWeb/wwwroot/Uploads/ImportJobWorkOpeningFormat.xlsx
+++ b/eTactWeb/wwwroot/Uploads/ImportJobWorkOpeningFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3F8888-B933-410E-BF9C-3E2CBE2AEB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD2AE08-7184-40CD-A607-91B819FBAA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
   <si>
     <t>ChallanNo</t>
   </si>
@@ -61,23 +61,113 @@
     <t>Uniqbatchno</t>
   </si>
   <si>
+    <t>DC905</t>
+  </si>
+  <si>
+    <t>RM0000378</t>
+  </si>
+  <si>
+    <t>RM0000362</t>
+  </si>
+  <si>
+    <t>RM0000194</t>
+  </si>
+  <si>
+    <t>RM0000448</t>
+  </si>
+  <si>
+    <t>RM0000169</t>
+  </si>
+  <si>
+    <t>RM0000093</t>
+  </si>
+  <si>
+    <t>RM0000383</t>
+  </si>
+  <si>
+    <t>RM0000257</t>
+  </si>
+  <si>
+    <t>RM0000367</t>
+  </si>
+  <si>
+    <t>RM0000322</t>
+  </si>
+  <si>
+    <t>RM0000013</t>
+  </si>
+  <si>
+    <t>RM0000315</t>
+  </si>
+  <si>
+    <t>RM0000382</t>
+  </si>
+  <si>
+    <t>RM0000062</t>
+  </si>
+  <si>
+    <t>RM0000179</t>
+  </si>
+  <si>
+    <t>RM0000011</t>
+  </si>
+  <si>
+    <t>RM0000237</t>
+  </si>
+  <si>
+    <t>RM0000420</t>
+  </si>
+  <si>
+    <t>RM0000030</t>
+  </si>
+  <si>
+    <t>RM0000327</t>
+  </si>
+  <si>
+    <t>RM0000267</t>
+  </si>
+  <si>
+    <t>RM0000012</t>
+  </si>
+  <si>
+    <t>RM0000423</t>
+  </si>
+  <si>
+    <t>RM0000115</t>
+  </si>
+  <si>
+    <t>RM0000116</t>
+  </si>
+  <si>
+    <t>RM0000413</t>
+  </si>
+  <si>
+    <t>RM0000324</t>
+  </si>
+  <si>
+    <t>RM0000249</t>
+  </si>
+  <si>
+    <t>RM0000246</t>
+  </si>
+  <si>
+    <t>NOS</t>
+  </si>
+  <si>
+    <t>JOB WORK</t>
+  </si>
+  <si>
+    <t>BATCH1</t>
+  </si>
+  <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>111HU00003</t>
-  </si>
-  <si>
-    <t>BMR</t>
-  </si>
-  <si>
-    <t>FGAL00001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,16 +175,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,13 +213,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,94 +584,1248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45778</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
-        <v>200</v>
-      </c>
-      <c r="F2">
-        <v>150</v>
-      </c>
-      <c r="G2">
+      <c r="E2" s="4">
+        <v>3706</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3706</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1962</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1962</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1470</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1470</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1295</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1295</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1073</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1073</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2255</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2255</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4195</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4195</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4">
+        <v>140</v>
+      </c>
+      <c r="F9" s="4">
+        <v>140</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3973</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3973</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4">
+        <v>499</v>
+      </c>
+      <c r="F11" s="4">
+        <v>499</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1597</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1597</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5">
+        <v>117</v>
+      </c>
+      <c r="F13" s="5">
+        <v>117</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="5">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5">
+        <v>34</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5">
+        <v>210</v>
+      </c>
+      <c r="F15" s="5">
+        <v>210</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="5">
+        <v>985</v>
+      </c>
+      <c r="F16" s="5">
+        <v>985</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E17" s="5">
+        <v>87</v>
+      </c>
+      <c r="F17" s="5">
+        <v>87</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="5">
+        <v>36</v>
+      </c>
+      <c r="F18" s="5">
+        <v>36</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="5">
+        <v>35</v>
+      </c>
+      <c r="F19" s="5">
+        <v>35</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="5">
+        <v>50</v>
+      </c>
+      <c r="F20" s="5">
+        <v>50</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5">
+        <v>414</v>
+      </c>
+      <c r="F21" s="5">
+        <v>414</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="5">
+        <v>173</v>
+      </c>
+      <c r="F22" s="5">
+        <v>173</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="5">
+        <v>620</v>
+      </c>
+      <c r="F23" s="5">
+        <v>620</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="5">
+        <v>28</v>
+      </c>
+      <c r="F24" s="5">
+        <v>28</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="5">
+        <v>142</v>
+      </c>
+      <c r="F25" s="5">
+        <v>142</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>22</v>
-      </c>
-      <c r="M2">
-        <v>22</v>
+      <c r="E26" s="5">
+        <v>943</v>
+      </c>
+      <c r="F26" s="5">
+        <v>943</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="5">
+        <v>557</v>
+      </c>
+      <c r="F27" s="5">
+        <v>557</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="5">
+        <v>3952</v>
+      </c>
+      <c r="F28" s="5">
+        <v>3952</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="5">
+        <v>585</v>
+      </c>
+      <c r="F29" s="5">
+        <v>585</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45741</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="5">
+        <v>3800</v>
+      </c>
+      <c r="F30" s="5">
+        <v>3800</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>